<commit_message>
Conc-Allgather is working and results are gathered
</commit_message>
<xml_diff>
--- a/MVAPICH/Results/NoleLand/NewSystem/Concurrent-Collectives/Conc_Bcast/NS-ConcBcast-MVAPICH.xlsx
+++ b/MVAPICH/Results/NoleLand/NewSystem/Concurrent-Collectives/Conc_Bcast/NS-ConcBcast-MVAPICH.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Default" sheetId="1" state="visible" r:id="rId2"/>
@@ -402,8 +402,8 @@
   </sheetPr>
   <dimension ref="A1:J859"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A109" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B121" activeCellId="0" sqref="B121"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A93" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H4" activeCellId="0" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5292,8 +5292,8 @@
   </sheetPr>
   <dimension ref="A1:J859"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D26" activeCellId="0" sqref="D26"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A115" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H4" activeCellId="0" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -10180,10 +10180,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E888"/>
+  <dimension ref="A1:G888"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G29" activeCellId="0" sqref="G29"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G12" activeCellId="0" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -10229,199 +10229,309 @@
       <c r="A5" s="16" t="n">
         <v>1</v>
       </c>
-      <c r="B5" s="17"/>
-      <c r="C5" s="17"/>
+      <c r="B5" s="17" t="n">
+        <v>2.244</v>
+      </c>
+      <c r="C5" s="17" t="n">
+        <v>6.21</v>
+      </c>
       <c r="D5" s="6"/>
       <c r="E5" s="2"/>
+      <c r="G5" s="0"/>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="16" t="n">
         <v>2</v>
       </c>
-      <c r="B6" s="17"/>
-      <c r="C6" s="17"/>
+      <c r="B6" s="17" t="n">
+        <v>1.816</v>
+      </c>
+      <c r="C6" s="17" t="n">
+        <v>5.638</v>
+      </c>
       <c r="D6" s="6"/>
       <c r="E6" s="2"/>
+      <c r="G6" s="0"/>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="16" t="n">
         <v>4</v>
       </c>
-      <c r="B7" s="17"/>
-      <c r="C7" s="17"/>
+      <c r="B7" s="17" t="n">
+        <v>1.812</v>
+      </c>
+      <c r="C7" s="17" t="n">
+        <v>5.562</v>
+      </c>
       <c r="D7" s="6"/>
       <c r="E7" s="2"/>
+      <c r="G7" s="0"/>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="16" t="n">
         <v>8</v>
       </c>
-      <c r="B8" s="17"/>
-      <c r="C8" s="17"/>
+      <c r="B8" s="17" t="n">
+        <v>1.816</v>
+      </c>
+      <c r="C8" s="17" t="n">
+        <v>5.564</v>
+      </c>
       <c r="D8" s="6"/>
       <c r="E8" s="2"/>
+      <c r="G8" s="0"/>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="16" t="n">
         <v>16</v>
       </c>
-      <c r="B9" s="17"/>
-      <c r="C9" s="17"/>
+      <c r="B9" s="17" t="n">
+        <v>1.808</v>
+      </c>
+      <c r="C9" s="17" t="n">
+        <v>5.508</v>
+      </c>
       <c r="D9" s="6"/>
       <c r="E9" s="2"/>
+      <c r="G9" s="0"/>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="16" t="n">
         <v>32</v>
       </c>
-      <c r="B10" s="17"/>
-      <c r="C10" s="17"/>
+      <c r="B10" s="17" t="n">
+        <v>1.852</v>
+      </c>
+      <c r="C10" s="17" t="n">
+        <v>5.564</v>
+      </c>
       <c r="D10" s="6"/>
       <c r="E10" s="2"/>
+      <c r="G10" s="0"/>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="16" t="n">
         <v>64</v>
       </c>
-      <c r="B11" s="17"/>
-      <c r="C11" s="17"/>
+      <c r="B11" s="17" t="n">
+        <v>1.894</v>
+      </c>
+      <c r="C11" s="17" t="n">
+        <v>5.9</v>
+      </c>
       <c r="D11" s="6"/>
       <c r="E11" s="2"/>
+      <c r="G11" s="0"/>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="16" t="n">
         <v>128</v>
       </c>
-      <c r="B12" s="17"/>
-      <c r="C12" s="17"/>
+      <c r="B12" s="17" t="n">
+        <v>1.95</v>
+      </c>
+      <c r="C12" s="17" t="n">
+        <v>5.964</v>
+      </c>
       <c r="D12" s="6"/>
       <c r="E12" s="2"/>
+      <c r="G12" s="0"/>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="16" t="n">
         <v>256</v>
       </c>
-      <c r="B13" s="17"/>
-      <c r="C13" s="17"/>
+      <c r="B13" s="17" t="n">
+        <v>2.258</v>
+      </c>
+      <c r="C13" s="17" t="n">
+        <v>5.976</v>
+      </c>
       <c r="D13" s="6"/>
       <c r="E13" s="2"/>
+      <c r="G13" s="0"/>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="16" t="n">
         <v>512</v>
       </c>
-      <c r="B14" s="17"/>
-      <c r="C14" s="17"/>
+      <c r="B14" s="17" t="n">
+        <v>2.45</v>
+      </c>
+      <c r="C14" s="17" t="n">
+        <v>6.188</v>
+      </c>
       <c r="D14" s="6"/>
       <c r="E14" s="2"/>
+      <c r="G14" s="0"/>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="16" t="n">
         <v>1024</v>
       </c>
-      <c r="B15" s="18"/>
-      <c r="C15" s="18"/>
+      <c r="B15" s="18" t="n">
+        <v>2.666</v>
+      </c>
+      <c r="C15" s="18" t="n">
+        <v>6.548</v>
+      </c>
       <c r="D15" s="6"/>
       <c r="E15" s="2"/>
+      <c r="G15" s="0"/>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="16" t="n">
         <v>2048</v>
       </c>
-      <c r="B16" s="18"/>
-      <c r="C16" s="18"/>
+      <c r="B16" s="18" t="n">
+        <v>3.254</v>
+      </c>
+      <c r="C16" s="18" t="n">
+        <v>7.954</v>
+      </c>
       <c r="D16" s="6"/>
       <c r="E16" s="2"/>
+      <c r="G16" s="0"/>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="16" t="n">
         <v>4096</v>
       </c>
-      <c r="B17" s="18"/>
-      <c r="C17" s="18"/>
+      <c r="B17" s="18" t="n">
+        <v>4.38</v>
+      </c>
+      <c r="C17" s="18" t="n">
+        <v>8.748</v>
+      </c>
       <c r="D17" s="6"/>
       <c r="E17" s="2"/>
+      <c r="G17" s="0"/>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="16" t="n">
         <v>8192</v>
       </c>
-      <c r="B18" s="18"/>
-      <c r="C18" s="18"/>
+      <c r="B18" s="18" t="n">
+        <v>6.288</v>
+      </c>
+      <c r="C18" s="18" t="n">
+        <v>10.85</v>
+      </c>
       <c r="D18" s="6"/>
       <c r="E18" s="2"/>
+      <c r="G18" s="0"/>
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="16" t="n">
         <v>16384</v>
       </c>
-      <c r="B19" s="18"/>
-      <c r="C19" s="18"/>
+      <c r="B19" s="18" t="n">
+        <v>8.49</v>
+      </c>
+      <c r="C19" s="18" t="n">
+        <v>13.48</v>
+      </c>
       <c r="D19" s="6"/>
       <c r="E19" s="2"/>
+      <c r="G19" s="0"/>
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="16" t="n">
         <v>32768</v>
       </c>
-      <c r="B20" s="18"/>
-      <c r="C20" s="18"/>
+      <c r="B20" s="18" t="n">
+        <v>13.282</v>
+      </c>
+      <c r="C20" s="18" t="n">
+        <v>22.432</v>
+      </c>
       <c r="D20" s="6"/>
       <c r="E20" s="2"/>
+      <c r="G20" s="0"/>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="16" t="n">
         <v>65536</v>
       </c>
-      <c r="B21" s="18"/>
-      <c r="C21" s="18"/>
+      <c r="B21" s="18" t="n">
+        <v>18.44</v>
+      </c>
+      <c r="C21" s="18" t="n">
+        <v>30.542</v>
+      </c>
       <c r="D21" s="6"/>
       <c r="E21" s="2"/>
+      <c r="G21" s="0"/>
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="16" t="n">
         <v>131072</v>
       </c>
-      <c r="B22" s="18"/>
-      <c r="C22" s="18"/>
+      <c r="B22" s="18" t="n">
+        <v>29.448</v>
+      </c>
+      <c r="C22" s="18" t="n">
+        <v>57.472</v>
+      </c>
       <c r="D22" s="6"/>
       <c r="E22" s="2"/>
+      <c r="G22" s="0"/>
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="16" t="n">
         <v>262144</v>
       </c>
-      <c r="B23" s="18"/>
-      <c r="C23" s="18"/>
+      <c r="B23" s="18" t="n">
+        <v>51.06</v>
+      </c>
+      <c r="C23" s="18" t="n">
+        <v>98.284</v>
+      </c>
       <c r="D23" s="6"/>
       <c r="E23" s="2"/>
+      <c r="G23" s="0"/>
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="16" t="n">
         <v>524288</v>
       </c>
-      <c r="B24" s="18"/>
-      <c r="C24" s="18"/>
+      <c r="B24" s="18" t="n">
+        <v>97.414</v>
+      </c>
+      <c r="C24" s="18" t="n">
+        <v>271.696</v>
+      </c>
       <c r="D24" s="6"/>
       <c r="E24" s="2"/>
+      <c r="G24" s="0"/>
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="16" t="n">
         <v>1048576</v>
       </c>
-      <c r="B25" s="18"/>
-      <c r="C25" s="18"/>
+      <c r="B25" s="18" t="n">
+        <v>226.786</v>
+      </c>
+      <c r="C25" s="18" t="n">
+        <v>514.916</v>
+      </c>
       <c r="D25" s="6"/>
       <c r="E25" s="2"/>
+      <c r="G25" s="0"/>
     </row>
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="16" t="n">
         <v>2097152</v>
       </c>
-      <c r="B26" s="18"/>
-      <c r="C26" s="18"/>
+      <c r="B26" s="18" t="n">
+        <v>470.198</v>
+      </c>
+      <c r="C26" s="18" t="n">
+        <v>1031.606</v>
+      </c>
       <c r="D26" s="6"/>
       <c r="E26" s="2"/>
+      <c r="G26" s="0"/>
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="6"/>
@@ -10471,183 +10581,293 @@
       <c r="A33" s="16" t="n">
         <v>1</v>
       </c>
-      <c r="B33" s="17"/>
-      <c r="C33" s="17"/>
+      <c r="B33" s="17" t="n">
+        <v>1.44</v>
+      </c>
+      <c r="C33" s="17" t="n">
+        <v>6.714</v>
+      </c>
       <c r="D33" s="6"/>
     </row>
     <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="16" t="n">
         <v>2</v>
       </c>
-      <c r="B34" s="17"/>
-      <c r="C34" s="17"/>
+      <c r="B34" s="17" t="n">
+        <v>1.032</v>
+      </c>
+      <c r="C34" s="17" t="n">
+        <v>6.228</v>
+      </c>
       <c r="D34" s="6"/>
+      <c r="G34" s="0"/>
     </row>
     <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="16" t="n">
         <v>4</v>
       </c>
-      <c r="B35" s="17"/>
-      <c r="C35" s="17"/>
+      <c r="B35" s="17" t="n">
+        <v>1.03</v>
+      </c>
+      <c r="C35" s="17" t="n">
+        <v>6.082</v>
+      </c>
       <c r="D35" s="6"/>
+      <c r="G35" s="0"/>
     </row>
     <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="16" t="n">
         <v>8</v>
       </c>
-      <c r="B36" s="17"/>
-      <c r="C36" s="17"/>
+      <c r="B36" s="17" t="n">
+        <v>1.028</v>
+      </c>
+      <c r="C36" s="17" t="n">
+        <v>6.04</v>
+      </c>
       <c r="D36" s="6"/>
+      <c r="G36" s="0"/>
     </row>
     <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="16" t="n">
         <v>16</v>
       </c>
-      <c r="B37" s="17"/>
-      <c r="C37" s="17"/>
+      <c r="B37" s="17" t="n">
+        <v>1.028</v>
+      </c>
+      <c r="C37" s="17" t="n">
+        <v>5.87</v>
+      </c>
       <c r="D37" s="6"/>
+      <c r="G37" s="0"/>
     </row>
     <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="16" t="n">
         <v>32</v>
       </c>
-      <c r="B38" s="17"/>
-      <c r="C38" s="17"/>
+      <c r="B38" s="17" t="n">
+        <v>1.062</v>
+      </c>
+      <c r="C38" s="17" t="n">
+        <v>6.046</v>
+      </c>
       <c r="D38" s="6"/>
+      <c r="G38" s="0"/>
     </row>
     <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="16" t="n">
         <v>64</v>
       </c>
-      <c r="B39" s="17"/>
-      <c r="C39" s="17"/>
+      <c r="B39" s="17" t="n">
+        <v>1.08</v>
+      </c>
+      <c r="C39" s="17" t="n">
+        <v>6.146</v>
+      </c>
       <c r="D39" s="6"/>
+      <c r="G39" s="0"/>
     </row>
     <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="16" t="n">
         <v>128</v>
       </c>
-      <c r="B40" s="17"/>
-      <c r="C40" s="17"/>
+      <c r="B40" s="17" t="n">
+        <v>1.132</v>
+      </c>
+      <c r="C40" s="17" t="n">
+        <v>7.038</v>
+      </c>
       <c r="D40" s="6"/>
+      <c r="G40" s="0"/>
     </row>
     <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="16" t="n">
         <v>256</v>
       </c>
-      <c r="B41" s="17"/>
-      <c r="C41" s="17"/>
+      <c r="B41" s="17" t="n">
+        <v>1.6</v>
+      </c>
+      <c r="C41" s="17" t="n">
+        <v>7.14</v>
+      </c>
       <c r="D41" s="6"/>
+      <c r="G41" s="0"/>
     </row>
     <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="16" t="n">
         <v>512</v>
       </c>
-      <c r="B42" s="17"/>
-      <c r="C42" s="17"/>
+      <c r="B42" s="17" t="n">
+        <v>1.856</v>
+      </c>
+      <c r="C42" s="17" t="n">
+        <v>7.324</v>
+      </c>
       <c r="D42" s="6"/>
+      <c r="G42" s="0"/>
     </row>
     <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="16" t="n">
         <v>1024</v>
       </c>
-      <c r="B43" s="18"/>
-      <c r="C43" s="18"/>
+      <c r="B43" s="18" t="n">
+        <v>2.094</v>
+      </c>
+      <c r="C43" s="18" t="n">
+        <v>7.82</v>
+      </c>
       <c r="D43" s="6"/>
+      <c r="G43" s="0"/>
     </row>
     <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="16" t="n">
         <v>2048</v>
       </c>
-      <c r="B44" s="18"/>
-      <c r="C44" s="18"/>
+      <c r="B44" s="18" t="n">
+        <v>3.394</v>
+      </c>
+      <c r="C44" s="18" t="n">
+        <v>9.39</v>
+      </c>
       <c r="D44" s="6"/>
+      <c r="G44" s="0"/>
     </row>
     <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="16" t="n">
         <v>4096</v>
       </c>
-      <c r="B45" s="18"/>
-      <c r="C45" s="18"/>
+      <c r="B45" s="18" t="n">
+        <v>4.842</v>
+      </c>
+      <c r="C45" s="18" t="n">
+        <v>10.59</v>
+      </c>
       <c r="D45" s="6"/>
+      <c r="G45" s="0"/>
     </row>
     <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="16" t="n">
         <v>8192</v>
       </c>
-      <c r="B46" s="18"/>
-      <c r="C46" s="18"/>
+      <c r="B46" s="18" t="n">
+        <v>6.474</v>
+      </c>
+      <c r="C46" s="18" t="n">
+        <v>12.97</v>
+      </c>
       <c r="D46" s="6"/>
+      <c r="G46" s="0"/>
     </row>
     <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="16" t="n">
         <v>16384</v>
       </c>
-      <c r="B47" s="18"/>
-      <c r="C47" s="18"/>
+      <c r="B47" s="18" t="n">
+        <v>9.94</v>
+      </c>
+      <c r="C47" s="18" t="n">
+        <v>19.572</v>
+      </c>
       <c r="D47" s="6"/>
+      <c r="G47" s="0"/>
     </row>
     <row r="48" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="16" t="n">
         <v>32768</v>
       </c>
-      <c r="B48" s="18"/>
-      <c r="C48" s="18"/>
+      <c r="B48" s="18" t="n">
+        <v>18.46</v>
+      </c>
+      <c r="C48" s="18" t="n">
+        <v>26.216</v>
+      </c>
       <c r="D48" s="6"/>
+      <c r="G48" s="0"/>
     </row>
     <row r="49" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="16" t="n">
         <v>65536</v>
       </c>
-      <c r="B49" s="18"/>
-      <c r="C49" s="18"/>
+      <c r="B49" s="18" t="n">
+        <v>25.2</v>
+      </c>
+      <c r="C49" s="18" t="n">
+        <v>46.986</v>
+      </c>
       <c r="D49" s="6"/>
+      <c r="G49" s="0"/>
     </row>
     <row r="50" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="16" t="n">
         <v>131072</v>
       </c>
-      <c r="B50" s="18"/>
-      <c r="C50" s="18"/>
+      <c r="B50" s="18" t="n">
+        <v>37.782</v>
+      </c>
+      <c r="C50" s="18" t="n">
+        <v>78.372</v>
+      </c>
       <c r="D50" s="6"/>
+      <c r="G50" s="0"/>
     </row>
     <row r="51" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="16" t="n">
         <v>262144</v>
       </c>
-      <c r="B51" s="18"/>
-      <c r="C51" s="18"/>
+      <c r="B51" s="18" t="n">
+        <v>69.352</v>
+      </c>
+      <c r="C51" s="18" t="n">
+        <v>148.404</v>
+      </c>
       <c r="D51" s="6"/>
+      <c r="G51" s="0"/>
     </row>
     <row r="52" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="16" t="n">
         <v>524288</v>
       </c>
-      <c r="B52" s="18"/>
-      <c r="C52" s="18"/>
+      <c r="B52" s="18" t="n">
+        <v>244.19</v>
+      </c>
+      <c r="C52" s="18" t="n">
+        <v>248.828</v>
+      </c>
       <c r="D52" s="6"/>
+      <c r="G52" s="0"/>
     </row>
     <row r="53" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A53" s="16" t="n">
         <v>1048576</v>
       </c>
-      <c r="B53" s="18"/>
-      <c r="C53" s="18"/>
+      <c r="B53" s="18" t="n">
+        <v>311.336</v>
+      </c>
+      <c r="C53" s="18" t="n">
+        <v>628.416</v>
+      </c>
       <c r="D53" s="6"/>
+      <c r="G53" s="0"/>
     </row>
     <row r="54" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="16" t="n">
         <v>2097152</v>
       </c>
-      <c r="B54" s="18"/>
-      <c r="C54" s="18"/>
+      <c r="B54" s="18" t="n">
+        <v>681.212</v>
+      </c>
+      <c r="C54" s="18" t="n">
+        <v>1415.09</v>
+      </c>
       <c r="D54" s="6"/>
+      <c r="G54" s="0"/>
     </row>
     <row r="55" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A55" s="6"/>
       <c r="B55" s="6"/>
       <c r="C55" s="6"/>
       <c r="D55" s="6"/>
+      <c r="G55" s="0"/>
     </row>
     <row r="56" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A56" s="6"/>
@@ -10691,189 +10911,299 @@
       <c r="A61" s="16" t="n">
         <v>1</v>
       </c>
-      <c r="B61" s="17"/>
-      <c r="C61" s="17"/>
+      <c r="B61" s="17" t="n">
+        <v>1.42</v>
+      </c>
+      <c r="C61" s="17" t="n">
+        <v>6.89</v>
+      </c>
       <c r="D61" s="6"/>
     </row>
     <row r="62" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A62" s="16" t="n">
         <v>2</v>
       </c>
-      <c r="B62" s="17"/>
-      <c r="C62" s="17"/>
+      <c r="B62" s="17" t="n">
+        <v>0.976</v>
+      </c>
+      <c r="C62" s="17" t="n">
+        <v>6.084</v>
+      </c>
       <c r="D62" s="6"/>
     </row>
     <row r="63" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A63" s="16" t="n">
         <v>4</v>
       </c>
-      <c r="B63" s="17"/>
-      <c r="C63" s="17"/>
+      <c r="B63" s="17" t="n">
+        <v>0.966</v>
+      </c>
+      <c r="C63" s="17" t="n">
+        <v>6.01</v>
+      </c>
       <c r="D63" s="6"/>
+      <c r="G63" s="0"/>
     </row>
     <row r="64" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A64" s="16" t="n">
         <v>8</v>
       </c>
-      <c r="B64" s="17"/>
-      <c r="C64" s="17"/>
+      <c r="B64" s="17" t="n">
+        <v>0.966</v>
+      </c>
+      <c r="C64" s="17" t="n">
+        <v>5.948</v>
+      </c>
       <c r="D64" s="6"/>
+      <c r="G64" s="0"/>
     </row>
     <row r="65" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A65" s="16" t="n">
         <v>16</v>
       </c>
-      <c r="B65" s="17"/>
-      <c r="C65" s="17"/>
+      <c r="B65" s="17" t="n">
+        <v>0.964</v>
+      </c>
+      <c r="C65" s="17" t="n">
+        <v>5.814</v>
+      </c>
       <c r="D65" s="6"/>
+      <c r="G65" s="0"/>
     </row>
     <row r="66" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A66" s="16" t="n">
         <v>32</v>
       </c>
-      <c r="B66" s="17"/>
-      <c r="C66" s="17"/>
+      <c r="B66" s="17" t="n">
+        <v>0.998</v>
+      </c>
+      <c r="C66" s="17" t="n">
+        <v>5.992</v>
+      </c>
       <c r="D66" s="6"/>
+      <c r="G66" s="0"/>
     </row>
     <row r="67" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A67" s="16" t="n">
         <v>64</v>
       </c>
-      <c r="B67" s="17"/>
-      <c r="C67" s="17"/>
+      <c r="B67" s="17" t="n">
+        <v>1.008</v>
+      </c>
+      <c r="C67" s="17" t="n">
+        <v>6.032</v>
+      </c>
       <c r="D67" s="6"/>
+      <c r="G67" s="0"/>
     </row>
     <row r="68" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A68" s="16" t="n">
         <v>128</v>
       </c>
-      <c r="B68" s="17"/>
-      <c r="C68" s="17"/>
+      <c r="B68" s="17" t="n">
+        <v>1.074</v>
+      </c>
+      <c r="C68" s="17" t="n">
+        <v>6.932</v>
+      </c>
       <c r="D68" s="6"/>
+      <c r="G68" s="0"/>
     </row>
     <row r="69" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A69" s="16" t="n">
         <v>256</v>
       </c>
-      <c r="B69" s="17"/>
-      <c r="C69" s="17"/>
+      <c r="B69" s="17" t="n">
+        <v>1.524</v>
+      </c>
+      <c r="C69" s="17" t="n">
+        <v>7.03</v>
+      </c>
       <c r="D69" s="6"/>
+      <c r="G69" s="0"/>
     </row>
     <row r="70" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A70" s="16" t="n">
         <v>512</v>
       </c>
-      <c r="B70" s="17"/>
-      <c r="C70" s="17"/>
+      <c r="B70" s="17" t="n">
+        <v>1.786</v>
+      </c>
+      <c r="C70" s="17" t="n">
+        <v>7.17</v>
+      </c>
       <c r="D70" s="6"/>
+      <c r="G70" s="0"/>
     </row>
     <row r="71" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A71" s="16" t="n">
         <v>1024</v>
       </c>
-      <c r="B71" s="18"/>
-      <c r="C71" s="18"/>
+      <c r="B71" s="18" t="n">
+        <v>2.042</v>
+      </c>
+      <c r="C71" s="18" t="n">
+        <v>7.75</v>
+      </c>
       <c r="D71" s="6"/>
+      <c r="G71" s="0"/>
     </row>
     <row r="72" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A72" s="16" t="n">
         <v>2048</v>
       </c>
-      <c r="B72" s="18"/>
-      <c r="C72" s="18"/>
+      <c r="B72" s="18" t="n">
+        <v>3.33</v>
+      </c>
+      <c r="C72" s="18" t="n">
+        <v>9.34</v>
+      </c>
       <c r="D72" s="6"/>
+      <c r="G72" s="0"/>
     </row>
     <row r="73" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A73" s="16" t="n">
         <v>4096</v>
       </c>
-      <c r="B73" s="18"/>
-      <c r="C73" s="18"/>
+      <c r="B73" s="18" t="n">
+        <v>4.8</v>
+      </c>
+      <c r="C73" s="18" t="n">
+        <v>10.592</v>
+      </c>
       <c r="D73" s="6"/>
+      <c r="G73" s="0"/>
     </row>
     <row r="74" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A74" s="16" t="n">
         <v>8192</v>
       </c>
-      <c r="B74" s="18"/>
-      <c r="C74" s="18"/>
+      <c r="B74" s="18" t="n">
+        <v>6.454</v>
+      </c>
+      <c r="C74" s="18" t="n">
+        <v>13</v>
+      </c>
       <c r="D74" s="6"/>
+      <c r="G74" s="0"/>
     </row>
     <row r="75" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A75" s="16" t="n">
         <v>16384</v>
       </c>
-      <c r="B75" s="18"/>
-      <c r="C75" s="18"/>
+      <c r="B75" s="18" t="n">
+        <v>9.452</v>
+      </c>
+      <c r="C75" s="18" t="n">
+        <v>19.558</v>
+      </c>
       <c r="D75" s="6"/>
+      <c r="G75" s="0"/>
     </row>
     <row r="76" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A76" s="16" t="n">
         <v>32768</v>
       </c>
-      <c r="B76" s="18"/>
-      <c r="C76" s="18"/>
+      <c r="B76" s="18" t="n">
+        <v>19.344</v>
+      </c>
+      <c r="C76" s="18" t="n">
+        <v>26.216</v>
+      </c>
       <c r="D76" s="6"/>
+      <c r="G76" s="0"/>
     </row>
     <row r="77" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A77" s="16" t="n">
         <v>65536</v>
       </c>
-      <c r="B77" s="18"/>
-      <c r="C77" s="18"/>
+      <c r="B77" s="18" t="n">
+        <v>25.372</v>
+      </c>
+      <c r="C77" s="18" t="n">
+        <v>47.428</v>
+      </c>
       <c r="D77" s="6"/>
+      <c r="G77" s="0"/>
     </row>
     <row r="78" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A78" s="16" t="n">
         <v>131072</v>
       </c>
-      <c r="B78" s="18"/>
-      <c r="C78" s="18"/>
+      <c r="B78" s="18" t="n">
+        <v>37.81</v>
+      </c>
+      <c r="C78" s="18" t="n">
+        <v>77.826</v>
+      </c>
       <c r="D78" s="6"/>
+      <c r="G78" s="0"/>
     </row>
     <row r="79" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A79" s="16" t="n">
         <v>262144</v>
       </c>
-      <c r="B79" s="18"/>
-      <c r="C79" s="18"/>
+      <c r="B79" s="18" t="n">
+        <v>69.186</v>
+      </c>
+      <c r="C79" s="18" t="n">
+        <v>149.324</v>
+      </c>
       <c r="D79" s="6"/>
+      <c r="G79" s="0"/>
     </row>
     <row r="80" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A80" s="16" t="n">
         <v>524288</v>
       </c>
-      <c r="B80" s="18"/>
-      <c r="C80" s="18"/>
+      <c r="B80" s="18" t="n">
+        <v>244.168</v>
+      </c>
+      <c r="C80" s="18" t="n">
+        <v>258.458</v>
+      </c>
       <c r="D80" s="6"/>
+      <c r="G80" s="0"/>
     </row>
     <row r="81" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A81" s="16" t="n">
         <v>1048576</v>
       </c>
-      <c r="B81" s="18"/>
-      <c r="C81" s="18"/>
+      <c r="B81" s="18" t="n">
+        <v>311.45</v>
+      </c>
+      <c r="C81" s="18" t="n">
+        <v>627.692</v>
+      </c>
       <c r="D81" s="6"/>
+      <c r="G81" s="0"/>
     </row>
     <row r="82" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A82" s="16" t="n">
         <v>2097152</v>
       </c>
-      <c r="B82" s="18"/>
-      <c r="C82" s="18"/>
+      <c r="B82" s="18" t="n">
+        <v>681.328</v>
+      </c>
+      <c r="C82" s="18" t="n">
+        <v>1409.044</v>
+      </c>
       <c r="D82" s="6"/>
+      <c r="G82" s="0"/>
     </row>
     <row r="83" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A83" s="6"/>
       <c r="B83" s="6"/>
       <c r="C83" s="6"/>
       <c r="D83" s="6"/>
+      <c r="G83" s="0"/>
     </row>
     <row r="84" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A84" s="6"/>
       <c r="B84" s="6"/>
       <c r="C84" s="6"/>
       <c r="D84" s="6"/>
+      <c r="G84" s="0"/>
     </row>
     <row r="85" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A85" s="6"/>
@@ -10911,195 +11241,305 @@
       <c r="A89" s="16" t="n">
         <v>1</v>
       </c>
-      <c r="B89" s="17"/>
-      <c r="C89" s="17"/>
+      <c r="B89" s="17" t="n">
+        <v>3.81</v>
+      </c>
+      <c r="C89" s="17" t="n">
+        <v>9.682</v>
+      </c>
       <c r="D89" s="6"/>
     </row>
     <row r="90" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A90" s="16" t="n">
         <v>2</v>
       </c>
-      <c r="B90" s="17"/>
-      <c r="C90" s="17"/>
+      <c r="B90" s="17" t="n">
+        <v>3.098</v>
+      </c>
+      <c r="C90" s="17" t="n">
+        <v>8.886</v>
+      </c>
       <c r="D90" s="6"/>
     </row>
     <row r="91" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A91" s="16" t="n">
         <v>4</v>
       </c>
-      <c r="B91" s="17"/>
-      <c r="C91" s="17"/>
+      <c r="B91" s="17" t="n">
+        <v>3.078</v>
+      </c>
+      <c r="C91" s="17" t="n">
+        <v>8.82</v>
+      </c>
       <c r="D91" s="6"/>
     </row>
     <row r="92" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A92" s="16" t="n">
         <v>8</v>
       </c>
-      <c r="B92" s="17"/>
-      <c r="C92" s="17"/>
+      <c r="B92" s="17" t="n">
+        <v>3.032</v>
+      </c>
+      <c r="C92" s="17" t="n">
+        <v>8.868</v>
+      </c>
       <c r="D92" s="6"/>
+      <c r="G92" s="0"/>
     </row>
     <row r="93" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A93" s="16" t="n">
         <v>16</v>
       </c>
-      <c r="B93" s="17"/>
-      <c r="C93" s="17"/>
+      <c r="B93" s="17" t="n">
+        <v>3.03</v>
+      </c>
+      <c r="C93" s="17" t="n">
+        <v>8.732</v>
+      </c>
       <c r="D93" s="6"/>
+      <c r="G93" s="0"/>
     </row>
     <row r="94" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A94" s="16" t="n">
         <v>32</v>
       </c>
-      <c r="B94" s="17"/>
-      <c r="C94" s="17"/>
+      <c r="B94" s="17" t="n">
+        <v>3.134</v>
+      </c>
+      <c r="C94" s="17" t="n">
+        <v>8.722</v>
+      </c>
       <c r="D94" s="6"/>
+      <c r="G94" s="0"/>
     </row>
     <row r="95" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A95" s="16" t="n">
         <v>64</v>
       </c>
-      <c r="B95" s="17"/>
-      <c r="C95" s="17"/>
+      <c r="B95" s="17" t="n">
+        <v>3.14</v>
+      </c>
+      <c r="C95" s="17" t="n">
+        <v>8.756</v>
+      </c>
       <c r="D95" s="6"/>
+      <c r="G95" s="0"/>
     </row>
     <row r="96" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A96" s="16" t="n">
         <v>128</v>
       </c>
-      <c r="B96" s="17"/>
-      <c r="C96" s="17"/>
+      <c r="B96" s="17" t="n">
+        <v>3.246</v>
+      </c>
+      <c r="C96" s="17" t="n">
+        <v>9.214</v>
+      </c>
       <c r="D96" s="6"/>
+      <c r="G96" s="0"/>
     </row>
     <row r="97" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A97" s="16" t="n">
         <v>256</v>
       </c>
-      <c r="B97" s="17"/>
-      <c r="C97" s="17"/>
+      <c r="B97" s="17" t="n">
+        <v>3.638</v>
+      </c>
+      <c r="C97" s="17" t="n">
+        <v>9.318</v>
+      </c>
       <c r="D97" s="6"/>
+      <c r="G97" s="0"/>
     </row>
     <row r="98" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A98" s="16" t="n">
         <v>512</v>
       </c>
-      <c r="B98" s="17"/>
-      <c r="C98" s="17"/>
+      <c r="B98" s="17" t="n">
+        <v>3.918</v>
+      </c>
+      <c r="C98" s="17" t="n">
+        <v>9.494</v>
+      </c>
       <c r="D98" s="6"/>
+      <c r="G98" s="0"/>
     </row>
     <row r="99" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A99" s="16" t="n">
         <v>1024</v>
       </c>
-      <c r="B99" s="18"/>
-      <c r="C99" s="18"/>
+      <c r="B99" s="18" t="n">
+        <v>4.2</v>
+      </c>
+      <c r="C99" s="18" t="n">
+        <v>9.884</v>
+      </c>
       <c r="D99" s="6"/>
+      <c r="G99" s="0"/>
     </row>
     <row r="100" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A100" s="16" t="n">
         <v>2048</v>
       </c>
-      <c r="B100" s="18"/>
-      <c r="C100" s="18"/>
+      <c r="B100" s="18" t="n">
+        <v>4.92</v>
+      </c>
+      <c r="C100" s="18" t="n">
+        <v>10.968</v>
+      </c>
       <c r="D100" s="6"/>
+      <c r="G100" s="0"/>
     </row>
     <row r="101" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A101" s="16" t="n">
         <v>4096</v>
       </c>
-      <c r="B101" s="18"/>
-      <c r="C101" s="18"/>
+      <c r="B101" s="18" t="n">
+        <v>6.624</v>
+      </c>
+      <c r="C101" s="18" t="n">
+        <v>13.226</v>
+      </c>
       <c r="D101" s="6"/>
+      <c r="G101" s="0"/>
     </row>
     <row r="102" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A102" s="16" t="n">
         <v>8192</v>
       </c>
-      <c r="B102" s="18"/>
-      <c r="C102" s="18"/>
+      <c r="B102" s="18" t="n">
+        <v>9.99</v>
+      </c>
+      <c r="C102" s="18" t="n">
+        <v>15.85</v>
+      </c>
       <c r="D102" s="6"/>
+      <c r="G102" s="0"/>
     </row>
     <row r="103" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A103" s="16" t="n">
         <v>16384</v>
       </c>
-      <c r="B103" s="18"/>
-      <c r="C103" s="18"/>
+      <c r="B103" s="18" t="n">
+        <v>13.082</v>
+      </c>
+      <c r="C103" s="18" t="n">
+        <v>20.59</v>
+      </c>
       <c r="D103" s="6"/>
+      <c r="G103" s="0"/>
     </row>
     <row r="104" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A104" s="16" t="n">
         <v>32768</v>
       </c>
-      <c r="B104" s="18"/>
-      <c r="C104" s="18"/>
+      <c r="B104" s="18" t="n">
+        <v>19.38</v>
+      </c>
+      <c r="C104" s="18" t="n">
+        <v>27.974</v>
+      </c>
       <c r="D104" s="6"/>
+      <c r="G104" s="0"/>
     </row>
     <row r="105" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A105" s="16" t="n">
         <v>65536</v>
       </c>
-      <c r="B105" s="18"/>
-      <c r="C105" s="18"/>
+      <c r="B105" s="18" t="n">
+        <v>28.78</v>
+      </c>
+      <c r="C105" s="18" t="n">
+        <v>50.818</v>
+      </c>
       <c r="D105" s="6"/>
+      <c r="G105" s="0"/>
     </row>
     <row r="106" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A106" s="16" t="n">
         <v>131072</v>
       </c>
-      <c r="B106" s="18"/>
-      <c r="C106" s="18"/>
+      <c r="B106" s="18" t="n">
+        <v>49.872</v>
+      </c>
+      <c r="C106" s="18" t="n">
+        <v>81.618</v>
+      </c>
       <c r="D106" s="6"/>
+      <c r="G106" s="0"/>
     </row>
     <row r="107" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A107" s="16" t="n">
         <v>262144</v>
       </c>
-      <c r="B107" s="18"/>
-      <c r="C107" s="18"/>
+      <c r="B107" s="18" t="n">
+        <v>75.212</v>
+      </c>
+      <c r="C107" s="18" t="n">
+        <v>120.66</v>
+      </c>
       <c r="D107" s="6"/>
+      <c r="G107" s="0"/>
     </row>
     <row r="108" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A108" s="16" t="n">
         <v>524288</v>
       </c>
-      <c r="B108" s="18"/>
-      <c r="C108" s="18"/>
+      <c r="B108" s="18" t="n">
+        <v>141.756</v>
+      </c>
+      <c r="C108" s="18" t="n">
+        <v>259.688</v>
+      </c>
       <c r="D108" s="6"/>
+      <c r="G108" s="0"/>
     </row>
     <row r="109" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A109" s="16" t="n">
         <v>1048576</v>
       </c>
-      <c r="B109" s="18"/>
-      <c r="C109" s="18"/>
+      <c r="B109" s="18" t="n">
+        <v>343.43</v>
+      </c>
+      <c r="C109" s="18" t="n">
+        <v>531.39</v>
+      </c>
       <c r="D109" s="6"/>
+      <c r="G109" s="0"/>
     </row>
     <row r="110" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A110" s="16" t="n">
         <v>2097152</v>
       </c>
-      <c r="B110" s="18"/>
-      <c r="C110" s="18"/>
+      <c r="B110" s="18" t="n">
+        <v>757.764</v>
+      </c>
+      <c r="C110" s="18" t="n">
+        <v>1223.676</v>
+      </c>
       <c r="D110" s="6"/>
+      <c r="G110" s="0"/>
     </row>
     <row r="111" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A111" s="6"/>
       <c r="B111" s="6"/>
       <c r="C111" s="6"/>
       <c r="D111" s="6"/>
+      <c r="G111" s="0"/>
     </row>
     <row r="112" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A112" s="6"/>
       <c r="B112" s="6"/>
       <c r="C112" s="6"/>
       <c r="D112" s="6"/>
+      <c r="G112" s="0"/>
     </row>
     <row r="113" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A113" s="6"/>
       <c r="B113" s="6"/>
       <c r="C113" s="6"/>
       <c r="D113" s="6"/>
+      <c r="G113" s="0"/>
     </row>
     <row r="114" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A114" s="11" t="s">
@@ -11131,201 +11571,311 @@
       <c r="A117" s="16" t="n">
         <v>1</v>
       </c>
-      <c r="B117" s="17"/>
-      <c r="C117" s="17"/>
+      <c r="B117" s="17" t="n">
+        <v>3.746</v>
+      </c>
+      <c r="C117" s="17" t="n">
+        <v>9.696</v>
+      </c>
       <c r="D117" s="6"/>
     </row>
     <row r="118" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A118" s="16" t="n">
         <v>2</v>
       </c>
-      <c r="B118" s="17"/>
-      <c r="C118" s="17"/>
+      <c r="B118" s="17" t="n">
+        <v>3.028</v>
+      </c>
+      <c r="C118" s="17" t="n">
+        <v>8.926</v>
+      </c>
       <c r="D118" s="6"/>
     </row>
     <row r="119" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A119" s="16" t="n">
         <v>4</v>
       </c>
-      <c r="B119" s="17"/>
-      <c r="C119" s="17"/>
+      <c r="B119" s="17" t="n">
+        <v>3.024</v>
+      </c>
+      <c r="C119" s="17" t="n">
+        <v>8.872</v>
+      </c>
       <c r="D119" s="6"/>
     </row>
     <row r="120" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A120" s="16" t="n">
         <v>8</v>
       </c>
-      <c r="B120" s="17"/>
-      <c r="C120" s="17"/>
+      <c r="B120" s="17" t="n">
+        <v>3.038</v>
+      </c>
+      <c r="C120" s="17" t="n">
+        <v>8.85</v>
+      </c>
       <c r="D120" s="6"/>
     </row>
     <row r="121" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A121" s="16" t="n">
         <v>16</v>
       </c>
-      <c r="B121" s="17"/>
-      <c r="C121" s="17"/>
+      <c r="B121" s="17" t="n">
+        <v>3.016</v>
+      </c>
+      <c r="C121" s="17" t="n">
+        <v>8.762</v>
+      </c>
       <c r="D121" s="6"/>
+      <c r="G121" s="0"/>
     </row>
     <row r="122" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A122" s="16" t="n">
         <v>32</v>
       </c>
-      <c r="B122" s="17"/>
-      <c r="C122" s="17"/>
+      <c r="B122" s="17" t="n">
+        <v>3.104</v>
+      </c>
+      <c r="C122" s="17" t="n">
+        <v>8.78</v>
+      </c>
       <c r="D122" s="6"/>
+      <c r="G122" s="0"/>
     </row>
     <row r="123" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A123" s="16" t="n">
         <v>64</v>
       </c>
-      <c r="B123" s="17"/>
-      <c r="C123" s="17"/>
+      <c r="B123" s="17" t="n">
+        <v>3.096</v>
+      </c>
+      <c r="C123" s="17" t="n">
+        <v>8.79</v>
+      </c>
       <c r="D123" s="6"/>
+      <c r="G123" s="0"/>
     </row>
     <row r="124" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A124" s="16" t="n">
         <v>128</v>
       </c>
-      <c r="B124" s="17"/>
-      <c r="C124" s="17"/>
+      <c r="B124" s="17" t="n">
+        <v>3.216</v>
+      </c>
+      <c r="C124" s="17" t="n">
+        <v>9.202</v>
+      </c>
       <c r="D124" s="6"/>
+      <c r="G124" s="0"/>
     </row>
     <row r="125" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A125" s="16" t="n">
         <v>256</v>
       </c>
-      <c r="B125" s="17"/>
-      <c r="C125" s="17"/>
+      <c r="B125" s="17" t="n">
+        <v>3.594</v>
+      </c>
+      <c r="C125" s="17" t="n">
+        <v>9.314</v>
+      </c>
       <c r="D125" s="6"/>
+      <c r="G125" s="0"/>
     </row>
     <row r="126" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A126" s="16" t="n">
         <v>512</v>
       </c>
-      <c r="B126" s="17"/>
-      <c r="C126" s="17"/>
+      <c r="B126" s="17" t="n">
+        <v>3.89</v>
+      </c>
+      <c r="C126" s="17" t="n">
+        <v>9.486</v>
+      </c>
       <c r="D126" s="6"/>
+      <c r="G126" s="0"/>
     </row>
     <row r="127" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A127" s="16" t="n">
         <v>1024</v>
       </c>
-      <c r="B127" s="18"/>
-      <c r="C127" s="18"/>
+      <c r="B127" s="18" t="n">
+        <v>4.178</v>
+      </c>
+      <c r="C127" s="18" t="n">
+        <v>9.868</v>
+      </c>
       <c r="D127" s="6"/>
+      <c r="G127" s="0"/>
     </row>
     <row r="128" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A128" s="16" t="n">
         <v>2048</v>
       </c>
-      <c r="B128" s="18"/>
-      <c r="C128" s="18"/>
+      <c r="B128" s="18" t="n">
+        <v>4.908</v>
+      </c>
+      <c r="C128" s="18" t="n">
+        <v>10.958</v>
+      </c>
       <c r="D128" s="6"/>
+      <c r="G128" s="0"/>
     </row>
     <row r="129" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A129" s="16" t="n">
         <v>4096</v>
       </c>
-      <c r="B129" s="18"/>
-      <c r="C129" s="18"/>
+      <c r="B129" s="18" t="n">
+        <v>6.674</v>
+      </c>
+      <c r="C129" s="18" t="n">
+        <v>13.312</v>
+      </c>
       <c r="D129" s="6"/>
+      <c r="G129" s="0"/>
     </row>
     <row r="130" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A130" s="16" t="n">
         <v>8192</v>
       </c>
-      <c r="B130" s="18"/>
-      <c r="C130" s="18"/>
+      <c r="B130" s="18" t="n">
+        <v>9.968</v>
+      </c>
+      <c r="C130" s="18" t="n">
+        <v>15.956</v>
+      </c>
       <c r="D130" s="6"/>
+      <c r="G130" s="0"/>
     </row>
     <row r="131" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A131" s="16" t="n">
         <v>16384</v>
       </c>
-      <c r="B131" s="18"/>
-      <c r="C131" s="18"/>
+      <c r="B131" s="18" t="n">
+        <v>13.086</v>
+      </c>
+      <c r="C131" s="18" t="n">
+        <v>20.826</v>
+      </c>
       <c r="D131" s="6"/>
+      <c r="G131" s="0"/>
     </row>
     <row r="132" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A132" s="16" t="n">
         <v>32768</v>
       </c>
-      <c r="B132" s="18"/>
-      <c r="C132" s="18"/>
+      <c r="B132" s="18" t="n">
+        <v>19.39</v>
+      </c>
+      <c r="C132" s="18" t="n">
+        <v>28.014</v>
+      </c>
       <c r="D132" s="6"/>
+      <c r="G132" s="0"/>
     </row>
     <row r="133" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A133" s="16" t="n">
         <v>65536</v>
       </c>
-      <c r="B133" s="18"/>
-      <c r="C133" s="18"/>
+      <c r="B133" s="18" t="n">
+        <v>28.518</v>
+      </c>
+      <c r="C133" s="18" t="n">
+        <v>50.836</v>
+      </c>
       <c r="D133" s="6"/>
+      <c r="G133" s="0"/>
     </row>
     <row r="134" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A134" s="16" t="n">
         <v>131072</v>
       </c>
-      <c r="B134" s="18"/>
-      <c r="C134" s="18"/>
+      <c r="B134" s="18" t="n">
+        <v>49.158</v>
+      </c>
+      <c r="C134" s="18" t="n">
+        <v>82.106</v>
+      </c>
       <c r="D134" s="6"/>
+      <c r="G134" s="0"/>
     </row>
     <row r="135" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A135" s="16" t="n">
         <v>262144</v>
       </c>
-      <c r="B135" s="18"/>
-      <c r="C135" s="18"/>
+      <c r="B135" s="18" t="n">
+        <v>74.238</v>
+      </c>
+      <c r="C135" s="18" t="n">
+        <v>125.206</v>
+      </c>
       <c r="D135" s="6"/>
+      <c r="G135" s="0"/>
     </row>
     <row r="136" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A136" s="16" t="n">
         <v>524288</v>
       </c>
-      <c r="B136" s="18"/>
-      <c r="C136" s="18"/>
+      <c r="B136" s="18" t="n">
+        <v>141.05</v>
+      </c>
+      <c r="C136" s="18" t="n">
+        <v>265.9</v>
+      </c>
       <c r="D136" s="6"/>
+      <c r="G136" s="0"/>
     </row>
     <row r="137" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A137" s="16" t="n">
         <v>1048576</v>
       </c>
-      <c r="B137" s="18"/>
-      <c r="C137" s="18"/>
+      <c r="B137" s="18" t="n">
+        <v>339.886</v>
+      </c>
+      <c r="C137" s="18" t="n">
+        <v>535.49</v>
+      </c>
       <c r="D137" s="6"/>
+      <c r="G137" s="0"/>
     </row>
     <row r="138" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A138" s="16" t="n">
         <v>2097152</v>
       </c>
-      <c r="B138" s="18"/>
-      <c r="C138" s="18"/>
+      <c r="B138" s="18" t="n">
+        <v>755.476</v>
+      </c>
+      <c r="C138" s="18" t="n">
+        <v>1215.204</v>
+      </c>
       <c r="D138" s="6"/>
+      <c r="G138" s="0"/>
     </row>
     <row r="139" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A139" s="6"/>
       <c r="B139" s="6"/>
       <c r="C139" s="6"/>
       <c r="D139" s="6"/>
+      <c r="G139" s="0"/>
     </row>
     <row r="140" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A140" s="6"/>
       <c r="B140" s="6"/>
       <c r="C140" s="6"/>
       <c r="D140" s="6"/>
+      <c r="G140" s="0"/>
     </row>
     <row r="141" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A141" s="6"/>
       <c r="B141" s="6"/>
       <c r="C141" s="6"/>
       <c r="D141" s="6"/>
+      <c r="G141" s="0"/>
     </row>
     <row r="142" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A142" s="6"/>
       <c r="B142" s="6"/>
       <c r="C142" s="6"/>
       <c r="D142" s="6"/>
+      <c r="G142" s="0"/>
     </row>
     <row r="143" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A143" s="6"/>

</xml_diff>